<commit_message>
Added functionality to calculate total sales between two dates, enabling detailed sales analysis over a specified period.
</commit_message>
<xml_diff>
--- a/beverage_sales.xlsx
+++ b/beverage_sales.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,6 +463,46 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>707d22be-52ec-4e60-8c20-5f4b21586443</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>s3Ida</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>7UP</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2024-09-15</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>01:19:17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>